<commit_message>
workin on email sender
</commit_message>
<xml_diff>
--- a/application/views/rpt/ua/LedgerPayments.xlsx
+++ b/application/views/rpt/ua/LedgerPayments.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\wamp\www\isell3\application\views\rpt\ua\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505"/>
   </bookViews>
@@ -66,9 +71,6 @@
     <t>{$v-&gt;p-&gt;company_name}, в особі __________________________________</t>
   </si>
   <si>
-    <t>з іншої сторони, склали цей акт звірки взаєморозрахунків за період з {$v-&gt;idate} за станом на {$v-&gt;fdate}.</t>
-  </si>
-  <si>
     <t>{$v-&gt;a-&gt;company_name}</t>
   </si>
   <si>
@@ -97,6 +99,9 @@
   </si>
   <si>
     <t>{$v-&gt;ledger-&gt;rows[]-&gt;trans_status}</t>
+  </si>
+  <si>
+    <t>з іншої сторони, склали цей акт звірки взаєморозрахунків за період з {$v-&gt;idate_dmy} за станом на {$v-&gt;fdate_dmy}.</t>
   </si>
 </sst>
 </file>
@@ -486,7 +491,7 @@
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -521,7 +526,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -733,7 +738,7 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:E4"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -773,7 +778,7 @@
     </row>
     <row r="4" spans="1:6" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B4" s="31" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="C4" s="31"/>
       <c r="D4" s="31"/>
@@ -803,7 +808,7 @@
       </c>
       <c r="C7" s="33"/>
       <c r="D7" s="28" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E7" s="28"/>
     </row>
@@ -826,22 +831,22 @@
     </row>
     <row r="9" spans="1:6" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" s="21" t="s">
         <v>25</v>
-      </c>
-      <c r="B9" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="D9" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="E9" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="F9" s="21" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -853,7 +858,7 @@
     </row>
     <row r="11" spans="1:6" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="34" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C11" s="34"/>
       <c r="D11" s="34"/>
@@ -861,7 +866,7 @@
     </row>
     <row r="12" spans="1:6" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B12" s="35" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C12" s="35"/>
       <c r="D12" s="35"/>
@@ -895,10 +900,10 @@
     </row>
     <row r="16" spans="1:6" s="2" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C16" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" s="25" t="s">
         <v>17</v>
-      </c>
-      <c r="D16" s="25" t="s">
-        <v>18</v>
       </c>
       <c r="E16" s="25"/>
     </row>

</xml_diff>